<commit_message>
Arreglado BNT pacientes mayores.
</commit_message>
<xml_diff>
--- a/TFG/res/pacientData/11006/Resultats_REM-G11006.xlsx
+++ b/TFG/res/pacientData/11006/Resultats_REM-G11006.xlsx
@@ -1838,61 +1838,61 @@
     <t>17</t>
   </si>
   <si>
-    <t>41-59</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t>29-40</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>252</t>
+  </si>
+  <si>
+    <t>0.96875</t>
+  </si>
+  <si>
+    <t>00:53.07</t>
+  </si>
+  <si>
+    <t>00:17.45</t>
+  </si>
+  <si>
+    <t>00:20.73</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>01:18.62</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>16.67</t>
+  </si>
+  <si>
+    <t>19.23</t>
+  </si>
+  <si>
+    <t>35.90</t>
   </si>
   <si>
     <t>11</t>
-  </si>
-  <si>
-    <t>128</t>
-  </si>
-  <si>
-    <t>57</t>
-  </si>
-  <si>
-    <t>21</t>
-  </si>
-  <si>
-    <t>-1</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>252</t>
-  </si>
-  <si>
-    <t>0.96875</t>
-  </si>
-  <si>
-    <t>00:53.07</t>
-  </si>
-  <si>
-    <t>00:17.45</t>
-  </si>
-  <si>
-    <t>00:20.73</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>01:18.62</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>22</t>
-  </si>
-  <si>
-    <t>16.67</t>
-  </si>
-  <si>
-    <t>19.23</t>
-  </si>
-  <si>
-    <t>35.90</t>
   </si>
   <si>
     <t>43</t>
@@ -4722,16 +4722,16 @@
         <v>607</v>
       </c>
       <c r="JM2" t="s">
-        <v>573</v>
+        <v>608</v>
       </c>
       <c r="JN2" t="s">
-        <v>576</v>
+        <v>582</v>
       </c>
       <c r="JO2" t="s">
+        <v>609</v>
+      </c>
+      <c r="JP2" t="s">
         <v>608</v>
-      </c>
-      <c r="JP2" t="s">
-        <v>609</v>
       </c>
       <c r="JQ2" t="s">
         <v>610</v>
@@ -4863,7 +4863,7 @@
         <v>558</v>
       </c>
       <c r="LH2" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="LI2" t="s">
         <v>567</v>
@@ -4884,19 +4884,19 @@
         <v>569</v>
       </c>
       <c r="LO2" t="s">
+        <v>622</v>
+      </c>
+      <c r="LP2" t="s">
         <v>623</v>
       </c>
-      <c r="LP2" t="s">
+      <c r="LQ2" t="s">
         <v>624</v>
       </c>
-      <c r="LQ2" t="s">
+      <c r="LR2" t="s">
         <v>625</v>
       </c>
-      <c r="LR2" t="s">
+      <c r="LS2" t="s">
         <v>626</v>
-      </c>
-      <c r="LS2" t="s">
-        <v>609</v>
       </c>
       <c r="LT2" t="s">
         <v>567</v>

</xml_diff>